<commit_message>
Se corrigio el Historial Académico
</commit_message>
<xml_diff>
--- a/web/resources/uploads/historial_academico.xlsx
+++ b/web/resources/uploads/historial_academico.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tincho\Projects\orion\web\resources\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C50A526-DC36-46ED-9F7D-74C76261F06F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29403B09-27BB-4D7B-8B6B-F86E9DCB8571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>CÓDIGO</t>
   </si>
@@ -177,6 +177,12 @@
   </si>
   <si>
     <t>&lt;&lt;RM_3&gt;&gt;</t>
+  </si>
+  <si>
+    <t>INSTITUTO:</t>
+  </si>
+  <si>
+    <t>&lt;&lt;INSTITUTO&gt;&gt;</t>
   </si>
 </sst>
 </file>
@@ -444,12 +450,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -461,9 +466,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -472,146 +474,153 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -951,7 +960,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:J30"/>
+  <dimension ref="A2:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
@@ -964,404 +973,424 @@
     <col min="5" max="5" width="48.5546875" customWidth="1"/>
     <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.44140625" customWidth="1"/>
-    <col min="8" max="8" width="6.6640625" style="17" customWidth="1"/>
+    <col min="8" max="8" width="6.6640625" style="14" customWidth="1"/>
     <col min="9" max="9" width="3.88671875" customWidth="1"/>
     <col min="10" max="10" width="16.77734375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="G2" s="29" t="s">
+      <c r="G2" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="24">
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="21">
         <v>-1</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
-    </row>
-    <row r="5" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="10"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="61"/>
+      <c r="J4" s="61"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="25"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="60" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="60"/>
+      <c r="C6" s="57" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="26"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="33"/>
-      <c r="C6" s="28">
+      <c r="B7" s="34"/>
+      <c r="C7" s="57">
         <v>-2</v>
       </c>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="5" t="s">
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="16"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="23" t="s">
+      <c r="H7" s="25"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="24" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="28" t="s">
+      <c r="B8" s="3"/>
+      <c r="C8" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="12" t="s">
+      <c r="D8" s="57"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="18"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="23" t="s">
+      <c r="H8" s="15"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="20" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="33" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="33"/>
-      <c r="C8" s="28" t="s">
+      <c r="B9" s="34"/>
+      <c r="C9" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="12" t="s">
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="H8" s="18"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="23" t="s">
+      <c r="H9" s="15"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="20" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="33" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="33"/>
-      <c r="C9" s="28" t="s">
+      <c r="B10" s="34"/>
+      <c r="C10" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="13"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="11"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="28" t="s">
+      <c r="B11" s="3"/>
+      <c r="C11" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="16"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+      <c r="D11" s="57"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="13"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="38" t="s">
+      <c r="C12" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-    </row>
-    <row r="12" spans="1:10" s="1" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="34" t="s">
+      <c r="D12" s="59"/>
+      <c r="E12" s="59"/>
+      <c r="F12" s="59"/>
+    </row>
+    <row r="13" spans="1:10" s="1" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B13" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="31" t="s">
+      <c r="C13" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="36" t="s">
+      <c r="D13" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="E12" s="60" t="s">
+      <c r="E13" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="31" t="s">
+      <c r="F13" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="G12" s="31" t="s">
+      <c r="G13" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="H12" s="31" t="s">
+      <c r="H13" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="I12" s="34" t="s">
+      <c r="I13" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="J12" s="34"/>
-    </row>
-    <row r="13" spans="1:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="34"/>
-      <c r="B13" s="37"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="61"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="3">
+      <c r="J13" s="35"/>
+    </row>
+    <row r="14" spans="1:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="35"/>
+      <c r="B14" s="51"/>
+      <c r="C14" s="55"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="58"/>
+      <c r="G14" s="55"/>
+      <c r="H14" s="55"/>
+      <c r="I14" s="35"/>
+      <c r="J14" s="35"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
         <v>-3</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="22" t="s">
+      <c r="E15" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="F14" s="26" t="s">
+      <c r="F15" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G15" s="2">
         <v>-50</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H15" s="2">
         <v>-51</v>
       </c>
-      <c r="I14" s="59" t="s">
+      <c r="I15" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="J14" s="59"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C15" s="6"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="7"/>
+      <c r="J15" s="49"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="9" t="s">
+      <c r="C16" s="5"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="6"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="7"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C17" s="6"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="7"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="6"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="21" t="s">
+      <c r="C18" s="5"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="6"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="6"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="21" t="s">
+      <c r="B19" s="5"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="6"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="21" t="s">
+      <c r="B20" s="5"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="B20" s="6"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H22" s="25"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="30" t="s">
+      <c r="B21" s="5"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H23" s="22"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="30"/>
-      <c r="C24" s="30"/>
-      <c r="D24" s="30"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="30"/>
-      <c r="H24" s="30"/>
-      <c r="I24" s="30"/>
-      <c r="J24" s="30"/>
-    </row>
-    <row r="26" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="47" t="s">
+      <c r="B25" s="56"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="56"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="56"/>
+      <c r="G25" s="56"/>
+      <c r="H25" s="56"/>
+      <c r="I25" s="56"/>
+      <c r="J25" s="56"/>
+    </row>
+    <row r="27" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="48"/>
-      <c r="D26" s="49"/>
-      <c r="E26" s="56" t="s">
+      <c r="C27" s="38"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="F26" s="57"/>
-      <c r="G26" s="40" t="s">
+      <c r="F27" s="47"/>
+      <c r="G27" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="H26" s="41"/>
-      <c r="I26" s="42"/>
-      <c r="J26" s="20">
+      <c r="H27" s="29"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="17">
         <v>3600</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="8" t="s">
+    <row r="28" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="45" t="s">
+      <c r="C28" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="D27" s="45"/>
-      <c r="E27" s="56"/>
-      <c r="F27" s="57"/>
-      <c r="G27" s="46" t="s">
+      <c r="D28" s="33"/>
+      <c r="E28" s="46"/>
+      <c r="F28" s="47"/>
+      <c r="G28" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="H27" s="46"/>
-      <c r="I27" s="46"/>
-      <c r="J27" s="3" t="s">
+      <c r="H28" s="36"/>
+      <c r="I28" s="36"/>
+      <c r="J28" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="14" t="s">
+    <row r="29" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="45" t="s">
+      <c r="C29" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="D28" s="45"/>
-      <c r="E28" s="56"/>
-      <c r="F28" s="57"/>
-      <c r="G28" s="50" t="s">
+      <c r="D29" s="33"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="47"/>
+      <c r="G29" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="H28" s="51"/>
-      <c r="I28" s="52"/>
-      <c r="J28" s="43">
+      <c r="H29" s="41"/>
+      <c r="I29" s="42"/>
+      <c r="J29" s="31">
         <v>-4</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="11">
+    <row r="30" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="9">
         <v>61</v>
       </c>
-      <c r="C29" s="58" t="s">
+      <c r="C30" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="D29" s="58"/>
-      <c r="E29" s="56"/>
-      <c r="F29" s="57"/>
-      <c r="G29" s="53"/>
-      <c r="H29" s="54"/>
-      <c r="I29" s="55"/>
-      <c r="J29" s="44"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B30" s="39" t="s">
+      <c r="D30" s="48"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="43"/>
+      <c r="H30" s="44"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="32"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B31" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="39"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="39"/>
-      <c r="G30" s="39"/>
-      <c r="H30" s="39"/>
-      <c r="I30" s="39"/>
-      <c r="J30" s="39"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="B30:J30"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="J28:J29"/>
-    <mergeCell ref="C27:D27"/>
+  <mergeCells count="34">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="A25:J25"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A9:B9"/>
-    <mergeCell ref="I12:J13"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="G28:I29"/>
-    <mergeCell ref="E26:F29"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="A24:J24"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C12:F12"/>
     <mergeCell ref="C7:F7"/>
     <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="B31:J31"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="J29:J30"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="I13:J14"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="G29:I30"/>
+    <mergeCell ref="E27:F30"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="H13:H14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>